<commit_message>
Input date was improved
</commit_message>
<xml_diff>
--- a/Examples/bev_lk.xlsx
+++ b/Examples/bev_lk.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1613" uniqueCount="1203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="1226">
   <si>
     <t>Key</t>
   </si>
@@ -3629,6 +3629,75 @@
   </si>
   <si>
     <t>DEG0M</t>
+  </si>
+  <si>
+    <t>SK Berlin Mitte</t>
+  </si>
+  <si>
+    <t>Bezirk</t>
+  </si>
+  <si>
+    <t>11002</t>
+  </si>
+  <si>
+    <t>11003</t>
+  </si>
+  <si>
+    <t>11004</t>
+  </si>
+  <si>
+    <t>11005</t>
+  </si>
+  <si>
+    <t>11006</t>
+  </si>
+  <si>
+    <t>11007</t>
+  </si>
+  <si>
+    <t>11008</t>
+  </si>
+  <si>
+    <t>SK Berlin Neukölln</t>
+  </si>
+  <si>
+    <t>SK Berlin Tempelhof-Schöneberg</t>
+  </si>
+  <si>
+    <t>SK Berlin Friedrichshain-Kreuzberg</t>
+  </si>
+  <si>
+    <t>SK Berlin Pankow</t>
+  </si>
+  <si>
+    <t>11010</t>
+  </si>
+  <si>
+    <t>SK Berli n Marzahl-Hellersdorf</t>
+  </si>
+  <si>
+    <t>SK Berlin Charlottenburg-Wilmersdorf</t>
+  </si>
+  <si>
+    <t>SK Berlin Spandau</t>
+  </si>
+  <si>
+    <t>SK Berlin Steglitz-Zehlendorf</t>
+  </si>
+  <si>
+    <t>11011</t>
+  </si>
+  <si>
+    <t>11012</t>
+  </si>
+  <si>
+    <t>SK Berlin Lichtenberg</t>
+  </si>
+  <si>
+    <t>SK Berlin Treptow-Köpenick</t>
+  </si>
+  <si>
+    <t>SK Berlin Reinickendorf</t>
   </si>
 </sst>
 </file>
@@ -3641,7 +3710,7 @@
     <numFmt numFmtId="166" formatCode="#&quot; &quot;###&quot; &quot;###&quot; &quot;##0"/>
     <numFmt numFmtId="167" formatCode="&quot; &quot;###&quot; &quot;####0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -3658,6 +3727,19 @@
       <color indexed="8"/>
       <name val="MetaNormalLF-Roman"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3673,7 +3755,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -3741,11 +3823,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3772,8 +3866,12 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4964,14 +5062,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV546"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A399" workbookViewId="0">
+      <selection activeCell="A419" sqref="A419:XFD419"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="27" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.21875" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
     <col min="7" max="8" width="15.44140625" style="1" customWidth="1"/>
@@ -20659,7 +20759,7 @@
       <c r="S402" s="4"/>
     </row>
     <row r="403" spans="1:19" ht="15" customHeight="1">
-      <c r="A403" s="4"/>
+      <c r="A403" s="5"/>
       <c r="B403" s="4"/>
       <c r="C403" s="4"/>
       <c r="D403" s="4"/>
@@ -20680,15 +20780,29 @@
       <c r="S403" s="4"/>
     </row>
     <row r="404" spans="1:19" ht="15" customHeight="1">
-      <c r="A404" s="4"/>
-      <c r="B404" s="4"/>
-      <c r="C404" s="4"/>
+      <c r="A404" s="5">
+        <v>11001</v>
+      </c>
+      <c r="B404" s="4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C404" s="4" t="s">
+        <v>1203</v>
+      </c>
       <c r="D404" s="4"/>
-      <c r="E404" s="9"/>
-      <c r="F404" s="4"/>
-      <c r="G404" s="4"/>
-      <c r="H404" s="4"/>
-      <c r="I404" s="4"/>
+      <c r="E404" s="9">
+        <v>10.69</v>
+      </c>
+      <c r="F404" s="10">
+        <v>384172</v>
+      </c>
+      <c r="G404" s="10">
+        <v>199188</v>
+      </c>
+      <c r="H404" s="10">
+        <v>184984</v>
+      </c>
+      <c r="I404" s="10"/>
       <c r="J404" s="4"/>
       <c r="K404" s="4"/>
       <c r="L404" s="4"/>
@@ -20701,15 +20815,29 @@
       <c r="S404" s="4"/>
     </row>
     <row r="405" spans="1:19" ht="15" customHeight="1">
-      <c r="A405" s="4"/>
-      <c r="B405" s="4"/>
-      <c r="C405" s="4"/>
+      <c r="A405" s="5" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B405" s="4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C405" s="4" t="s">
+        <v>1214</v>
+      </c>
       <c r="D405" s="4"/>
-      <c r="E405" s="9"/>
-      <c r="F405" s="4"/>
-      <c r="G405" s="4"/>
-      <c r="H405" s="4"/>
-      <c r="I405" s="4"/>
+      <c r="E405" s="9">
+        <v>20.2</v>
+      </c>
+      <c r="F405" s="10">
+        <v>289762</v>
+      </c>
+      <c r="G405" s="10">
+        <v>148927</v>
+      </c>
+      <c r="H405" s="10">
+        <v>140835</v>
+      </c>
+      <c r="I405" s="10"/>
       <c r="J405" s="4"/>
       <c r="K405" s="4"/>
       <c r="L405" s="4"/>
@@ -20722,15 +20850,29 @@
       <c r="S405" s="4"/>
     </row>
     <row r="406" spans="1:19" ht="15" customHeight="1">
-      <c r="A406" s="4"/>
-      <c r="B406" s="4"/>
-      <c r="C406" s="4"/>
+      <c r="A406" s="5" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B406" s="4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C406" s="4" t="s">
+        <v>1215</v>
+      </c>
       <c r="D406" s="4"/>
-      <c r="E406" s="9"/>
-      <c r="F406" s="4"/>
-      <c r="G406" s="4"/>
-      <c r="H406" s="4"/>
-      <c r="I406" s="4"/>
+      <c r="E406" s="9">
+        <v>103.07</v>
+      </c>
+      <c r="F406" s="10">
+        <v>407765</v>
+      </c>
+      <c r="G406" s="10">
+        <v>200304</v>
+      </c>
+      <c r="H406" s="10">
+        <v>207461</v>
+      </c>
+      <c r="I406" s="10"/>
       <c r="J406" s="4"/>
       <c r="K406" s="4"/>
       <c r="L406" s="4"/>
@@ -20743,15 +20885,29 @@
       <c r="S406" s="4"/>
     </row>
     <row r="407" spans="1:19" ht="15" customHeight="1">
-      <c r="A407" s="4"/>
-      <c r="B407" s="4"/>
-      <c r="C407" s="4"/>
+      <c r="A407" s="5" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B407" s="4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C407" s="4" t="s">
+        <v>1218</v>
+      </c>
       <c r="D407" s="4"/>
-      <c r="E407" s="9"/>
-      <c r="F407" s="4"/>
-      <c r="G407" s="4"/>
-      <c r="H407" s="4"/>
-      <c r="I407" s="4"/>
+      <c r="E407" s="9">
+        <v>64.7</v>
+      </c>
+      <c r="F407" s="10">
+        <v>342332</v>
+      </c>
+      <c r="G407" s="10">
+        <v>166124</v>
+      </c>
+      <c r="H407" s="10">
+        <v>176208</v>
+      </c>
+      <c r="I407" s="10"/>
       <c r="J407" s="4"/>
       <c r="K407" s="4"/>
       <c r="L407" s="4"/>
@@ -20764,15 +20920,29 @@
       <c r="S407" s="4"/>
     </row>
     <row r="408" spans="1:19" ht="15" customHeight="1">
-      <c r="A408" s="4"/>
-      <c r="B408" s="4"/>
-      <c r="C408" s="4"/>
+      <c r="A408" s="5" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B408" s="4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C408" s="4" t="s">
+        <v>1219</v>
+      </c>
       <c r="D408" s="4"/>
-      <c r="E408" s="9"/>
-      <c r="F408" s="4"/>
-      <c r="G408" s="4"/>
-      <c r="H408" s="4"/>
-      <c r="I408" s="4"/>
+      <c r="E408" s="9">
+        <v>91.878</v>
+      </c>
+      <c r="F408" s="10">
+        <v>243977</v>
+      </c>
+      <c r="G408" s="10">
+        <v>119445</v>
+      </c>
+      <c r="H408" s="10">
+        <v>124532</v>
+      </c>
+      <c r="I408" s="10"/>
       <c r="J408" s="4"/>
       <c r="K408" s="4"/>
       <c r="L408" s="4"/>
@@ -20785,15 +20955,29 @@
       <c r="S408" s="4"/>
     </row>
     <row r="409" spans="1:19" ht="15" customHeight="1">
-      <c r="A409" s="4"/>
-      <c r="B409" s="4"/>
-      <c r="C409" s="4"/>
+      <c r="A409" s="5" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B409" s="4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C409" s="4" t="s">
+        <v>1220</v>
+      </c>
       <c r="D409" s="4"/>
-      <c r="E409" s="9"/>
-      <c r="F409" s="4"/>
-      <c r="G409" s="4"/>
-      <c r="H409" s="4"/>
-      <c r="I409" s="4"/>
+      <c r="E409" s="9">
+        <v>102.5</v>
+      </c>
+      <c r="F409" s="10">
+        <v>308697</v>
+      </c>
+      <c r="G409" s="10">
+        <v>146203</v>
+      </c>
+      <c r="H409" s="10">
+        <v>162494</v>
+      </c>
+      <c r="I409" s="10"/>
       <c r="J409" s="4"/>
       <c r="K409" s="4"/>
       <c r="L409" s="4"/>
@@ -20806,15 +20990,29 @@
       <c r="S409" s="4"/>
     </row>
     <row r="410" spans="1:19" ht="15" customHeight="1">
-      <c r="A410" s="4"/>
-      <c r="B410" s="4"/>
-      <c r="C410" s="4"/>
+      <c r="A410" s="5" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B410" s="4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C410" s="4" t="s">
+        <v>1213</v>
+      </c>
       <c r="D410" s="4"/>
-      <c r="E410" s="9"/>
-      <c r="F410" s="4"/>
-      <c r="G410" s="4"/>
-      <c r="H410" s="4"/>
-      <c r="I410" s="4"/>
+      <c r="E410" s="9">
+        <v>53.09</v>
+      </c>
+      <c r="F410" s="10">
+        <v>351644</v>
+      </c>
+      <c r="G410" s="10">
+        <v>172377</v>
+      </c>
+      <c r="H410" s="10">
+        <v>179267</v>
+      </c>
+      <c r="I410" s="10"/>
       <c r="J410" s="4"/>
       <c r="K410" s="4"/>
       <c r="L410" s="4"/>
@@ -20827,15 +21025,29 @@
       <c r="S410" s="4"/>
     </row>
     <row r="411" spans="1:19" ht="15" customHeight="1">
-      <c r="A411" s="4"/>
-      <c r="B411" s="4"/>
-      <c r="C411" s="4"/>
+      <c r="A411" s="5" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B411" s="4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C411" s="4" t="s">
+        <v>1212</v>
+      </c>
       <c r="D411" s="4"/>
-      <c r="E411" s="9"/>
-      <c r="F411" s="4"/>
-      <c r="G411" s="4"/>
-      <c r="H411" s="4"/>
-      <c r="I411" s="4"/>
+      <c r="E411" s="9">
+        <v>44.9</v>
+      </c>
+      <c r="F411" s="10">
+        <v>329691</v>
+      </c>
+      <c r="G411" s="10">
+        <v>164423</v>
+      </c>
+      <c r="H411" s="10">
+        <v>165268</v>
+      </c>
+      <c r="I411" s="10"/>
       <c r="J411" s="4"/>
       <c r="K411" s="4"/>
       <c r="L411" s="4"/>
@@ -20848,15 +21060,29 @@
       <c r="S411" s="4"/>
     </row>
     <row r="412" spans="1:19" ht="15" customHeight="1">
-      <c r="A412" s="4"/>
-      <c r="B412" s="4"/>
-      <c r="C412" s="4"/>
+      <c r="A412" s="5">
+        <v>11009</v>
+      </c>
+      <c r="B412" s="4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C412" s="18" t="s">
+        <v>1224</v>
+      </c>
       <c r="D412" s="4"/>
-      <c r="E412" s="9"/>
-      <c r="F412" s="4"/>
-      <c r="G412" s="4"/>
-      <c r="H412" s="4"/>
-      <c r="I412" s="4"/>
+      <c r="E412" s="9">
+        <v>892</v>
+      </c>
+      <c r="F412" s="10">
+        <v>271153</v>
+      </c>
+      <c r="G412" s="10">
+        <v>132961</v>
+      </c>
+      <c r="H412" s="10">
+        <v>138192</v>
+      </c>
+      <c r="I412" s="10"/>
       <c r="J412" s="4"/>
       <c r="K412" s="4"/>
       <c r="L412" s="4"/>
@@ -20869,15 +21095,29 @@
       <c r="S412" s="4"/>
     </row>
     <row r="413" spans="1:19" ht="15" customHeight="1">
-      <c r="A413" s="4"/>
-      <c r="B413" s="4"/>
-      <c r="C413" s="4"/>
+      <c r="A413" s="5" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B413" s="4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C413" s="4" t="s">
+        <v>1217</v>
+      </c>
       <c r="D413" s="4"/>
-      <c r="E413" s="9"/>
-      <c r="F413" s="4"/>
-      <c r="G413" s="4"/>
-      <c r="H413" s="4"/>
-      <c r="I413" s="4"/>
+      <c r="E413" s="9">
+        <v>61.8</v>
+      </c>
+      <c r="F413" s="10">
+        <v>268548</v>
+      </c>
+      <c r="G413" s="10">
+        <v>133140</v>
+      </c>
+      <c r="H413" s="10">
+        <v>135408</v>
+      </c>
+      <c r="I413" s="10"/>
       <c r="J413" s="4"/>
       <c r="K413" s="4"/>
       <c r="L413" s="4"/>
@@ -20890,15 +21130,29 @@
       <c r="S413" s="4"/>
     </row>
     <row r="414" spans="1:19" ht="15" customHeight="1">
-      <c r="A414" s="4"/>
-      <c r="B414" s="4"/>
-      <c r="C414" s="4"/>
+      <c r="A414" s="5" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B414" s="4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C414" s="4" t="s">
+        <v>1223</v>
+      </c>
       <c r="D414" s="4"/>
-      <c r="E414" s="9"/>
-      <c r="F414" s="4"/>
-      <c r="G414" s="4"/>
-      <c r="H414" s="4"/>
-      <c r="I414" s="4"/>
+      <c r="E414" s="9">
+        <v>52.29</v>
+      </c>
+      <c r="F414" s="10">
+        <v>291452</v>
+      </c>
+      <c r="G414" s="10">
+        <v>144740</v>
+      </c>
+      <c r="H414" s="10">
+        <v>146712</v>
+      </c>
+      <c r="I414" s="10"/>
       <c r="J414" s="4"/>
       <c r="K414" s="4"/>
       <c r="L414" s="4"/>
@@ -20911,15 +21165,29 @@
       <c r="S414" s="4"/>
     </row>
     <row r="415" spans="1:19" ht="15" customHeight="1">
-      <c r="A415" s="4"/>
-      <c r="B415" s="4"/>
-      <c r="C415" s="4"/>
+      <c r="A415" s="5" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B415" s="4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C415" s="19" t="s">
+        <v>1225</v>
+      </c>
       <c r="D415" s="4"/>
-      <c r="E415" s="9"/>
-      <c r="F415" s="4"/>
-      <c r="G415" s="4"/>
-      <c r="H415" s="4"/>
-      <c r="I415" s="4"/>
+      <c r="E415" s="9">
+        <v>89.48</v>
+      </c>
+      <c r="F415" s="10">
+        <v>265225</v>
+      </c>
+      <c r="G415" s="10">
+        <v>130557</v>
+      </c>
+      <c r="H415" s="10">
+        <v>134668</v>
+      </c>
+      <c r="I415" s="10"/>
       <c r="J415" s="4"/>
       <c r="K415" s="4"/>
       <c r="L415" s="4"/>
@@ -20932,12 +21200,12 @@
       <c r="S415" s="4"/>
     </row>
     <row r="416" spans="1:19" ht="15" customHeight="1">
-      <c r="A416" s="4"/>
+      <c r="A416" s="5"/>
       <c r="B416" s="4"/>
       <c r="C416" s="4"/>
       <c r="D416" s="4"/>
       <c r="E416" s="9"/>
-      <c r="F416" s="4"/>
+      <c r="F416" s="10"/>
       <c r="G416" s="4"/>
       <c r="H416" s="4"/>
       <c r="I416" s="4"/>
@@ -20973,16 +21241,16 @@
       <c r="R417" s="4"/>
       <c r="S417" s="4"/>
     </row>
-    <row r="418" spans="1:19" ht="15" customHeight="1">
-      <c r="A418" s="4"/>
-      <c r="B418" s="4"/>
-      <c r="C418" s="4"/>
-      <c r="D418" s="4"/>
-      <c r="E418" s="9"/>
-      <c r="F418" s="4"/>
-      <c r="G418" s="4"/>
-      <c r="H418" s="4"/>
-      <c r="I418" s="4"/>
+    <row r="418" spans="1:19" ht="27" customHeight="1">
+      <c r="A418" s="2"/>
+      <c r="B418" s="2"/>
+      <c r="C418" s="3"/>
+      <c r="D418" s="2"/>
+      <c r="E418" s="2"/>
+      <c r="F418" s="2"/>
+      <c r="G418" s="2"/>
+      <c r="H418" s="2"/>
+      <c r="I418" s="2"/>
       <c r="J418" s="4"/>
       <c r="K418" s="4"/>
       <c r="L418" s="4"/>
@@ -20995,7 +21263,7 @@
       <c r="S418" s="4"/>
     </row>
     <row r="419" spans="1:19" ht="15" customHeight="1">
-      <c r="A419" s="4"/>
+      <c r="A419" s="20"/>
       <c r="B419" s="4"/>
       <c r="C419" s="4"/>
       <c r="D419" s="4"/>

</xml_diff>